<commit_message>
Finished back-end infrastructure, added registration page
</commit_message>
<xml_diff>
--- a/doc/Product Backlog.xlsx
+++ b/doc/Product Backlog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Github\Catch\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Github\Catch\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="9045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="9045" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product  backlog" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Sprint 1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product  backlog'!$A$1:$E$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product  backlog'!$A$1:$E$6</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -548,11 +548,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,143 +592,143 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>110</v>
-      </c>
-      <c r="D3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>11</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="B5">
+        <v>90</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B6">
+        <v>80</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>45</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>108</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="E8" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>40</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>35</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>8</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>100</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>90</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>80</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>50</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9">
-        <v>45</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>40</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>7</v>
-      </c>
       <c r="B11">
-        <v>35</v>
-      </c>
-      <c r="D11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>9</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>8</v>
-      </c>
       <c r="B12">
-        <v>25</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>16</v>
@@ -736,29 +736,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B14">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>19</v>
-      </c>
-      <c r="B15">
-        <v>20</v>
-      </c>
-      <c r="D15" s="3" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="17" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -792,9 +779,8 @@
     <row r="48" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:E7">
+  <autoFilter ref="A1:E6">
     <sortState ref="A2:F13">
       <sortCondition descending="1" ref="B1"/>
     </sortState>
@@ -812,7 +798,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,15 +855,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="48.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="61.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -965,9 +951,19 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+    <row r="7" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>110</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>